<commit_message>
Handled memo field on Origen Bank file
</commit_message>
<xml_diff>
--- a/OPIDDaily/Uploads/Voided Origen Checks.xlsx
+++ b/OPIDDaily/Uploads/Voided Origen Checks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apricot\OPID\Voided Checks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F79F341-E383-48B9-A0FC-E7E71C901998}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889B3C77-3131-4097-828E-6A9CEFD6EC1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33705" yWindow="1050" windowWidth="13830" windowHeight="6360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="4620" windowWidth="13830" windowHeight="6360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Voided Checks" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Type</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Green, Denita</t>
+  </si>
+  <si>
+    <t>Foo</t>
   </si>
 </sst>
 </file>
@@ -410,7 +413,7 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,6 +475,9 @@
       <c r="G2" t="s">
         <v>11</v>
       </c>
+      <c r="I2">
+        <v>39077</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -486,6 +492,9 @@
       <c r="G3" t="s">
         <v>11</v>
       </c>
+      <c r="I3">
+        <v>39078</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -500,6 +509,9 @@
       <c r="G4" t="s">
         <v>12</v>
       </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -509,10 +521,13 @@
         <v>44239</v>
       </c>
       <c r="E5">
-        <v>1067</v>
+        <v>1194</v>
       </c>
       <c r="G5" t="s">
         <v>13</v>
+      </c>
+      <c r="I5">
+        <v>39085</v>
       </c>
     </row>
   </sheetData>

</xml_diff>